<commit_message>
67763 Sprint1 Amend - Work Breakdown Structure corresponds directly to user stories and generated tasks
</commit_message>
<xml_diff>
--- a/SE202526/Management/Work_Breakdown_Structure.xlsx
+++ b/SE202526/Management/Work_Breakdown_Structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/059c692484dd0481/uni/Semestre5/ES/SE2526_67775_67804_67286_68130_68547_67763/SE202526/Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95229DF5-9C92-4D15-B70D-F0E92C4C89EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{95229DF5-9C92-4D15-B70D-F0E92C4C89EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD4AC7CC-BA18-4753-B925-830BFC96C11F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-9855" windowWidth="29040" windowHeight="15720" xr2:uid="{B7004714-AD48-4058-A71F-4BA2362B2B43}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12072" windowHeight="12336" xr2:uid="{B7004714-AD48-4058-A71F-4BA2362B2B43}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -96,16 +96,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>518264</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>26670</xdr:rowOff>
+      <xdr:rowOff>37108</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>125260</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:rowOff>117118</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -120,8 +120,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5524500" y="388620"/>
-          <a:ext cx="1181100" cy="984885"/>
+          <a:off x="5361661" y="412889"/>
+          <a:ext cx="1423270" cy="1019462"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -281,11 +281,11 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-GB" sz="1400"/>
-            <a:t>1.2.1</a:t>
+            <a:t>US3: Define </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1400" baseline="0"/>
-            <a:t> Official player experience (our own, Trello board)</a:t>
+            <a:t>3 new functionalities</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1400"/>
         </a:p>
@@ -485,11 +485,19 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-GB" sz="1400"/>
-            <a:t>1.1.1 Game</a:t>
+            <a:t>US1:</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1400" baseline="0"/>
-            <a:t> familiarisation</a:t>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400"/>
+            <a:t>General grasp of</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+            <a:t> game mechanics</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1400"/>
         </a:p>
@@ -553,11 +561,11 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-GB" sz="1400"/>
-            <a:t>1.1.2</a:t>
+            <a:t>US2:</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1400" baseline="0"/>
-            <a:t> Code familiarisation</a:t>
+            <a:t> Read the codebase</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1400"/>
         </a:p>
@@ -621,13 +629,8 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-GB" sz="1400"/>
-            <a:t>1.1.1.1 Playing the first</a:t>
+            <a:t>T1: Play the first area of the game</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
-            <a:t> map</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="1400"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -643,8 +646,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>167096</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>74295</xdr:rowOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>93946</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -659,8 +662,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3993425" y="7252607"/>
-          <a:ext cx="1684564" cy="958759"/>
+          <a:off x="3952044" y="7703507"/>
+          <a:ext cx="1663874" cy="1221288"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -689,18 +692,18 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-GB" sz="1400"/>
-            <a:t>1.1.2.1</a:t>
+            <a:t>T2:</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-GB" sz="1400"/>
-            <a:t>Surface-level</a:t>
+            <a:t>Read through the classes</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1400" baseline="0"/>
-            <a:t> code readthrough</a:t>
+            <a:t> in the codebase</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1400"/>
         </a:p>
@@ -710,16 +713,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>13606</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>4899</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>514647</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>171913</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>489855</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>385472</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>73208</xdr:rowOff>
+      <xdr:rowOff>52331</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -734,8 +737,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6749142" y="7257506"/>
-          <a:ext cx="1700892" cy="952773"/>
+          <a:off x="5963469" y="7687529"/>
+          <a:ext cx="1687099" cy="1007761"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -763,155 +766,15 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-GB" sz="1400"/>
-            <a:t>1.2.1</a:t>
-          </a:r>
-          <a:r>
             <a:rPr lang="en-GB" sz="1400" baseline="0"/>
-            <a:t>.1 Potential early game helpful features</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="1400"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>83548</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>22316</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>554082</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>108857</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="Rectangle: Rounded Corners 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F535318-F251-4391-9907-E75FBE7A624E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9268369" y="7274923"/>
-          <a:ext cx="1695177" cy="1147898"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400"/>
-            <a:t>1.2.1.2</a:t>
+            <a:t>T3:</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-GB" sz="1400" baseline="0"/>
-            <a:t>Group-assisted functionality brainstorming</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="1400"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>21227</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>81642</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>484141</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>124369</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="Rectangle: Rounded Corners 25">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEB5AB13-4A3E-4A9C-823E-1C4C9A13B484}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11655334" y="5565321"/>
-          <a:ext cx="1687557" cy="927191"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400"/>
-            <a:t>1.2.2</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
-            <a:t>Early functionality prototyping</a:t>
+            <a:t>Define roughly functionality 1</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1400"/>
         </a:p>
@@ -922,15 +785,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>19049</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>117117</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>21348</xdr:colOff>
+      <xdr:colOff>23140</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>169968</xdr:rowOff>
+      <xdr:rowOff>166157</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -948,8 +811,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="5820844" y="1699636"/>
-          <a:ext cx="616986" cy="2298"/>
+          <a:off x="5768986" y="1736660"/>
+          <a:ext cx="612711" cy="4091"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -1217,7 +1080,9 @@
           <a:ext cx="770165" cy="15511"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
-          <a:avLst/>
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 3194"/>
+          </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
@@ -1239,69 +1104,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>231183</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>146413</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>252683</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>81642</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="44" name="Connector: Elbow 43">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44FC0874-531A-78F9-69EF-3E9F91D470AC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="15" idx="2"/>
-          <a:endCxn id="26" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="10241551" y="3307759"/>
-          <a:ext cx="819694" cy="3695429"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>252685</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>147349</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>98516</xdr:rowOff>
+      <xdr:rowOff>102327</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>215674</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>6803</xdr:rowOff>
+      <xdr:colOff>218170</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>171913</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1319,8 +1131,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="7797982" y="6269219"/>
-          <a:ext cx="792751" cy="1187632"/>
+          <a:off x="7339994" y="6333408"/>
+          <a:ext cx="821147" cy="1887095"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -1346,15 +1158,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>215674</xdr:colOff>
+      <xdr:colOff>218168</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>98516</xdr:rowOff>
+      <xdr:rowOff>102327</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>317863</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>18505</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>285133</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>174000</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1366,14 +1178,15 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
           <a:stCxn id="6" idx="2"/>
-          <a:endCxn id="25" idx="0"/>
+          <a:endCxn id="10" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="9049363" y="6205470"/>
-          <a:ext cx="804453" cy="1326832"/>
+          <a:off x="9224116" y="6336379"/>
+          <a:ext cx="823234" cy="1883239"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -1452,15 +1265,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>544286</xdr:colOff>
+      <xdr:colOff>538932</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>553267</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>176892</xdr:rowOff>
+      <xdr:colOff>546008</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1478,8 +1291,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="4435657" y="6848746"/>
-          <a:ext cx="798739" cy="8981"/>
+          <a:off x="4352627" y="7272153"/>
+          <a:ext cx="855632" cy="7076"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -1557,16 +1370,15 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-GB" sz="1400"/>
-            <a:t>1.2.2.1</a:t>
+            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+            <a:t>T6:</a:t>
           </a:r>
-          <a:endParaRPr lang="en-GB" sz="1400" baseline="0"/>
         </a:p>
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-GB" sz="1400" baseline="0"/>
-            <a:t>Trial modification of the code</a:t>
+            <a:t>Trial modification of  code</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1400"/>
         </a:p>
@@ -1576,16 +1388,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>246969</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>218168</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>126273</xdr:rowOff>
+      <xdr:rowOff>102327</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>249827</xdr:colOff>
+      <xdr:colOff>250777</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>173081</xdr:rowOff>
+      <xdr:rowOff>176892</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1597,14 +1409,15 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="26" idx="2"/>
+          <a:cxnSpLocks/>
+          <a:stCxn id="6" idx="2"/>
           <a:endCxn id="58" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="12117637" y="6870177"/>
-          <a:ext cx="754379" cy="2858"/>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="10113629" y="5446866"/>
+          <a:ext cx="826126" cy="3665157"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -1625,6 +1438,148 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>51183</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>167737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>527433</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>48155</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle: Rounded Corners 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{796AA7D2-972D-452A-B464-0AFD9C7AE056}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7921704" y="7683353"/>
+          <a:ext cx="1687099" cy="1007761"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+            <a:t>T4: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+            <a:t>Define roughly functionality 2</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>47008</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>174000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>523258</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>54418</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle: Rounded Corners 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7AB6551-F4CF-4E90-9E02-0C136BD7020E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9733803" y="7689616"/>
+          <a:ext cx="1687099" cy="1007761"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+            <a:t>T5:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+            <a:t>Define roughly functionality 3</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1949,8 +1904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED716E8-F608-4006-B5DA-359448DC4BDE}">
   <dimension ref="A1:W49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+    <sheetView tabSelected="1" topLeftCell="G17" zoomScale="73" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>